<commit_message>
UPdate tao moi process
</commit_message>
<xml_diff>
--- a/angular/src/assets/SoYeuLyLich.xlsx
+++ b/angular/src/assets/SoYeuLyLich.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="30">
   <si>
     <t>Loại Tài Khoản</t>
   </si>
@@ -823,7 +823,7 @@
   <dimension ref="A1:M30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -831,11 +831,11 @@
     <col min="1" max="4" width="14.75" style="14" customWidth="1"/>
     <col min="5" max="5" width="15" style="11" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.625" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.625" style="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.25" style="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.5" style="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.25" style="14" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.625" style="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.625" style="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.625" style="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.25" style="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5" style="14" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.25" style="14" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.375" style="11" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="19" style="11" bestFit="1" customWidth="1"/>
     <col min="14" max="16384" width="14" style="11"/>
@@ -861,19 +861,19 @@
         <v>2</v>
       </c>
       <c r="G1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>12</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>4</v>
       </c>
       <c r="L1" s="5" t="s">
         <v>9</v>
@@ -902,19 +902,19 @@
         <v>15</v>
       </c>
       <c r="G2" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="I2" s="8" t="s">
         <v>23</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>20</v>
       </c>
       <c r="J2" s="8" t="s">
         <v>20</v>
       </c>
       <c r="K2" s="8" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="L2" s="9" t="s">
         <v>22</v>
@@ -925,18 +925,42 @@
     </row>
     <row r="3" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="9"/>
-      <c r="M3" s="10"/>
+      <c r="B3" s="8">
+        <v>1</v>
+      </c>
+      <c r="C3" s="8">
+        <v>1</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L3" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="M3" s="10" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="4" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
@@ -1376,7 +1400,7 @@
           <x14:formula1>
             <xm:f>GiaTri!$E$2:$E$3</xm:f>
           </x14:formula1>
-          <xm:sqref>K2:K29</xm:sqref>
+          <xm:sqref>G2:G29</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>